<commit_message>
Added mmol standardized biomass reactions
</commit_message>
<xml_diff>
--- a/data/13c_mfa/INCA_model_08302023_GR.xlsx
+++ b/data/13c_mfa/INCA_model_08302023_GR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrettroell/yarrowia_eflux2/data/13c_mfa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE4048F-3489-254E-A836-4F71F53DF5BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C049741E-BE89-5C47-B96A-CE8E0228B57F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1300" windowWidth="35840" windowHeight="18100" activeTab="4" xr2:uid="{F5B582E7-5936-49E8-BD16-34BCB0ED06A3}"/>
   </bookViews>
@@ -1497,7 +1497,7 @@
     <t>oleic_acid_UB</t>
   </si>
   <si>
-    <t>biomass_C or biomass_glucose or biomass_oleic_acid</t>
+    <t>biomass_C or biomass_glucose or biomass_oil</t>
   </si>
 </sst>
 </file>
@@ -12878,7 +12878,7 @@
   <dimension ref="A1:U74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>